<commit_message>
Add mobile app not in use data set
</commit_message>
<xml_diff>
--- a/Banking_Mobile_Application_Usage_Analysis_ETL_Data.xlsx
+++ b/Banking_Mobile_Application_Usage_Analysis_ETL_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\MSC\3RD-SEM\CS5651 - Statistical Inference\UOM_2020_CS5651_Statistical_Inference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E597DECD-1C92-4C24-9618-DAF57F1AA69E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6423C54-E8A2-469D-B550-FD2C2EA094C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-4740" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -1101,28 +1101,70 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B109" sqref="B109"/>
+    <sheetView tabSelected="1" topLeftCell="AY1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BJ3" sqref="BJ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="37" customWidth="1"/>
-    <col min="7" max="9" width="33.28515625" customWidth="1"/>
-    <col min="10" max="10" width="57.28515625" customWidth="1"/>
-    <col min="11" max="11" width="154.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="51" customWidth="1"/>
-    <col min="13" max="13" width="72.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="20" width="41.28515625" style="1" customWidth="1"/>
-    <col min="21" max="26" width="54.140625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="67.85546875" style="1" customWidth="1"/>
-    <col min="28" max="28" width="54.140625" style="1" customWidth="1"/>
-    <col min="29" max="29" width="54.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="54.5703125" customWidth="1"/>
-    <col min="31" max="31" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="3.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="26" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="57.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="51.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="20" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:59" x14ac:dyDescent="0.25">

</xml_diff>